<commit_message>
#85 fix specs and fixtures for new implementation
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/categories_table.xlsx
+++ b/spec/fixtures/files/categories_table.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Category Trees" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Demographics - SC" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Demographics" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="347">
   <si>
     <t xml:space="preserve">Standard Extract</t>
   </si>
@@ -383,10 +383,31 @@
     <t xml:space="preserve">Table includes all 'By Request' variables and 'Default' variables considered to be Demographic</t>
   </si>
   <si>
+    <t xml:space="preserve">Category (L0) == the standard extract</t>
+  </si>
+  <si>
     <t xml:space="preserve">Includes: Census (SC, AP, PRU, EYC) and Early Years, Primary, Secondary and KS5 Educational Phases </t>
   </si>
   <si>
     <t xml:space="preserve">Missing: Many default EYC and EYFSP variables, and many KS5 default variables</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category (L0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category (L0) Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category (L1) Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category (L2) Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category (L3) Description</t>
   </si>
   <si>
     <t xml:space="preserve">Concept level</t>
@@ -1050,7 +1071,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1081,26 +1102,61 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1119,8 +1175,20 @@
         <bgColor rgb="FFE2F0D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1235,6 +1303,48 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
@@ -1266,7 +1376,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="112">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1471,15 +1581,231 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1487,7 +1813,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1496,78 +1822,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1650,8 +1904,8 @@
   </sheetPr>
   <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C97" activeCellId="0" sqref="C97"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C97" activeCellId="0" sqref="A1:Y184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2482,10 +2736,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U186"/>
+  <dimension ref="A1:Y186"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N25" activeCellId="0" sqref="N25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Y184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2501,1601 +2755,2188 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="8.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H1" s="51"/>
+      <c r="I1" s="51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="K5" s="0" t="s">
+      <c r="H5" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="I5" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="J5" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="K5" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="L5" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="M5" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="N5" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="R5" s="0" t="s">
+      <c r="O5" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="S5" s="0" t="s">
+      <c r="P5" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="Q5" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="U5" s="0" t="s">
+      <c r="R5" s="57" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="52" t="s">
+      <c r="S5" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="T5" s="57" t="s">
+        <v>140</v>
+      </c>
+      <c r="U5" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="V5" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="W5" s="57" t="s">
+        <v>143</v>
+      </c>
+      <c r="X5" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y5" s="57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="59"/>
+      <c r="C6" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="54" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="55"/>
-      <c r="E7" s="54" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55"/>
-      <c r="E8" s="54" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="55"/>
-      <c r="E9" s="54" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="57" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="55"/>
-      <c r="B11" s="58" t="s">
+      <c r="D6" s="61"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="58"/>
+      <c r="B7" s="64"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="58"/>
+      <c r="B8" s="64"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="58"/>
+      <c r="B9" s="64"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="58"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="58"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="70"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="72" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55"/>
-      <c r="B12" s="59" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="58"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61" t="s">
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="76" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="55"/>
-      <c r="E13" s="54" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55"/>
-      <c r="E14" s="54" t="s">
-        <v>145</v>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="58"/>
+      <c r="B13" s="64"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="63" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="58"/>
+      <c r="B14" s="64"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="55"/>
-      <c r="E15" s="54" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="55"/>
-      <c r="B17" s="61" t="s">
+      <c r="A15" s="58"/>
+      <c r="B15" s="64"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="58"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="58"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="D17" s="78"/>
+      <c r="E17" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55"/>
-      <c r="B18" s="54"/>
-      <c r="E18" s="54" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="55"/>
-      <c r="B19" s="54"/>
-      <c r="E19" s="54" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="55"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="57" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="55"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="53" t="s">
+      <c r="F17" s="74"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="58"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="80"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="63" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="58"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="80"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="58"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="58"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="55"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="55"/>
-      <c r="B23" s="61" t="s">
+      <c r="F21" s="74"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="58"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="58"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="D23" s="85"/>
+      <c r="E23" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="61" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="G23" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="H23" s="62" t="s">
-        <v>157</v>
-      </c>
-      <c r="I23" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="J23" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="K23" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="L23" s="62" t="s">
+      <c r="F23" s="74"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="76" t="s">
         <v>161</v>
       </c>
-      <c r="M23" s="65" t="s">
+      <c r="J23" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="N23" s="66" t="s">
+      <c r="K23" s="86" t="s">
         <v>163</v>
       </c>
-      <c r="O23" s="66" t="s">
+      <c r="L23" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="P23" s="66" t="s">
+      <c r="M23" s="87" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55"/>
-      <c r="B24" s="54"/>
-      <c r="E24" s="54" t="s">
+      <c r="N23" s="88" t="s">
         <v>166</v>
       </c>
-      <c r="G24" s="62" t="s">
+      <c r="O23" s="88" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="55"/>
-      <c r="B25" s="54"/>
-      <c r="E25" s="54" t="s">
+      <c r="P23" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="G25" s="62" t="s">
+      <c r="Q23" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="R23" s="90" t="s">
         <v>170</v>
       </c>
+      <c r="S23" s="90" t="s">
+        <v>171</v>
+      </c>
+      <c r="T23" s="90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="58"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="64"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="K24" s="86" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="19.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="58"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="64"/>
+      <c r="H25" s="62"/>
       <c r="I25" s="63" t="s">
-        <v>171</v>
-      </c>
-      <c r="J25" s="63" t="s">
-        <v>172</v>
-      </c>
-      <c r="K25" s="64" t="s">
-        <v>173</v>
-      </c>
-      <c r="L25" s="64" t="s">
-        <v>174</v>
-      </c>
-      <c r="M25" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="N25" s="66" t="s">
+      <c r="K25" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="O25" s="63" t="s">
+      <c r="L25" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="P25" s="63" t="s">
+      <c r="M25" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="Q25" s="62" t="s">
+      <c r="N25" s="87" t="s">
         <v>179</v>
       </c>
-      <c r="R25" s="62" t="s">
+      <c r="O25" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="S25" s="63" t="s">
+      <c r="P25" s="88" t="s">
         <v>181</v>
       </c>
-      <c r="T25" s="63" t="s">
+      <c r="Q25" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="U25" s="63" t="s">
+      <c r="R25" s="90" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="57" t="s">
+      <c r="S25" s="87" t="s">
         <v>184</v>
       </c>
-      <c r="G26" s="63" t="s">
+      <c r="T25" s="87" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="55"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="53" t="s">
+      <c r="U25" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="V25" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="W25" s="87" t="s">
+        <v>188</v>
+      </c>
+      <c r="X25" s="87" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y25" s="87" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="58"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="K26" s="87" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="58"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="E27" s="54" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="55"/>
-      <c r="B28" s="54"/>
-      <c r="E28" s="54" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="55"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="57" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="55"/>
-      <c r="B30" s="61" t="s">
+      <c r="F27" s="74"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="63" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="58"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="64"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="58"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="58"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="D30" s="91"/>
+      <c r="E30" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="61" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="55"/>
-      <c r="B31" s="54"/>
-      <c r="E31" s="54" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55"/>
-      <c r="B32" s="54"/>
-      <c r="E32" s="54" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="55"/>
-      <c r="B33" s="54"/>
-      <c r="E33" s="54" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="55"/>
-      <c r="B34" s="54"/>
-      <c r="E34" s="54" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="55"/>
-      <c r="B35" s="54"/>
-      <c r="E35" s="54" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="55"/>
-      <c r="B36" s="54"/>
-      <c r="E36" s="54" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="55"/>
-      <c r="B37" s="54"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="54" t="s">
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="76" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="55"/>
-      <c r="B38" s="54"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="54" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="58"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="64"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="63" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="55"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="57" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="58"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="64"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="63" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="55"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="59" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="58"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="64"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="63" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="58"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="64"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="63" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="58"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="64"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="63" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="58"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="64"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="63" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="58"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="64"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="63" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="58"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="64"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="63" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="58"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="58"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="55"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="57" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="55"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="59" t="s">
+      <c r="F40" s="74"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="76" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="58"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+      <c r="I41" s="67" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="58"/>
+      <c r="B42" s="65"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="55"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="53"/>
-      <c r="E43" s="54" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="55"/>
-      <c r="B44" s="54"/>
-      <c r="E44" s="54" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="55"/>
-      <c r="B45" s="54"/>
-      <c r="E45" s="54" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="55"/>
-      <c r="B46" s="54"/>
-      <c r="E46" s="54" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="55"/>
-      <c r="B47" s="54"/>
-      <c r="E47" s="54" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="55"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="57" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="55"/>
-      <c r="B49" s="54"/>
-      <c r="C49" s="59" t="s">
+      <c r="F42" s="74"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="76" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="58"/>
+      <c r="B43" s="65"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="60"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="58"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="64"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="63" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="58"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="64"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="63" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="58"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="64"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="63" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="58"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="64"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="63" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="58"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+      <c r="I48" s="67" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="58"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="60"/>
-      <c r="E49" s="61" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="55"/>
-      <c r="B50" s="54"/>
-      <c r="E50" s="54" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="55"/>
-      <c r="B51" s="54"/>
-      <c r="E51" s="54" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="55"/>
-      <c r="B52" s="54"/>
-      <c r="E52" s="54" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="55"/>
-      <c r="B53" s="54"/>
-      <c r="E53" s="54" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="55"/>
-      <c r="B54" s="54"/>
-      <c r="E54" s="54" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="55"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="57" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="55"/>
-      <c r="B56" s="54"/>
-      <c r="C56" s="58" t="s">
+      <c r="F49" s="74"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="76" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="58"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="64"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="58"/>
+      <c r="B51" s="65"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="64"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="63" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="58"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="64"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="63" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="58"/>
+      <c r="B53" s="65"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="64"/>
+      <c r="H53" s="62"/>
+      <c r="I53" s="63" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="58"/>
+      <c r="B54" s="65"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="64"/>
+      <c r="H54" s="62"/>
+      <c r="I54" s="63" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="58"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="65"/>
+      <c r="E55" s="66"/>
+      <c r="F55" s="66"/>
+      <c r="G55" s="66"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="67" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="58"/>
+      <c r="B56" s="65"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="68"/>
+      <c r="E56" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="55"/>
-      <c r="B57" s="54"/>
-      <c r="C57" s="59" t="s">
+      <c r="F56" s="74"/>
+      <c r="G56" s="71"/>
+      <c r="H56" s="71"/>
+      <c r="I56" s="72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="58"/>
+      <c r="B57" s="65"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="55"/>
-      <c r="B58" s="54"/>
-      <c r="E58" s="54" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="55"/>
-      <c r="B59" s="54"/>
-      <c r="E59" s="0" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="55"/>
-      <c r="B60" s="54"/>
-      <c r="E60" s="54" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="55"/>
-      <c r="B61" s="54"/>
-      <c r="E61" s="54" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="55"/>
-      <c r="B62" s="54"/>
-      <c r="E62" s="54" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="55"/>
-      <c r="B63" s="54"/>
-      <c r="E63" s="54" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="55"/>
-      <c r="B64" s="54"/>
-      <c r="E64" s="54" t="s">
+      <c r="F57" s="74"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
+      <c r="I57" s="76" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="55"/>
-      <c r="B65" s="54"/>
-      <c r="E65" s="54" t="s">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="58"/>
+      <c r="B58" s="65"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="64"/>
+      <c r="H58" s="62"/>
+      <c r="I58" s="63" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="55"/>
-      <c r="B66" s="54"/>
-      <c r="E66" s="54" t="s">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="58"/>
+      <c r="B59" s="65"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="64"/>
+      <c r="I59" s="92" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="55"/>
-      <c r="B67" s="54"/>
-      <c r="E67" s="54" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="58"/>
+      <c r="B60" s="65"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="64"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="63" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="55"/>
-      <c r="B68" s="54"/>
-      <c r="E68" s="54" t="s">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="58"/>
+      <c r="B61" s="65"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="64"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="63" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="55"/>
-      <c r="B69" s="54"/>
-      <c r="E69" s="54" t="s">
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="58"/>
+      <c r="B62" s="65"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="64"/>
+      <c r="H62" s="62"/>
+      <c r="I62" s="63" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="55"/>
-      <c r="B70" s="54"/>
-      <c r="E70" s="54" t="s">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="58"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="64"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="63" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="55"/>
-      <c r="B71" s="54"/>
-      <c r="E71" s="54" t="s">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="58"/>
+      <c r="B64" s="65"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="64"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="63" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="55"/>
-      <c r="B72" s="54"/>
-      <c r="E72" s="54" t="s">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="58"/>
+      <c r="B65" s="65"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="64"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="63" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="55"/>
-      <c r="B73" s="54"/>
-      <c r="E73" s="54" t="s">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="58"/>
+      <c r="B66" s="65"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="64"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="63" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="55"/>
-      <c r="B74" s="54"/>
-      <c r="E74" s="54" t="s">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="58"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="64"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="63" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="55"/>
-      <c r="B75" s="57"/>
-      <c r="C75" s="56"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="57" t="s">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="58"/>
+      <c r="B68" s="65"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="64"/>
+      <c r="H68" s="62"/>
+      <c r="I68" s="63" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="55"/>
-      <c r="B76" s="59" t="s">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="58"/>
+      <c r="B69" s="65"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="64"/>
+      <c r="H69" s="62"/>
+      <c r="I69" s="63" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="58"/>
+      <c r="B70" s="65"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="64"/>
+      <c r="H70" s="62"/>
+      <c r="I70" s="63" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="58"/>
+      <c r="B71" s="65"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="64"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="63" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="58"/>
+      <c r="B72" s="65"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="64"/>
+      <c r="H72" s="62"/>
+      <c r="I72" s="63" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="58"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="64"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="63" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="58"/>
+      <c r="B74" s="65"/>
+      <c r="C74" s="62"/>
+      <c r="D74" s="64"/>
+      <c r="H74" s="62"/>
+      <c r="I74" s="63" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="58"/>
+      <c r="B75" s="65"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="93"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="66"/>
+      <c r="I75" s="67" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="58"/>
+      <c r="B76" s="68"/>
+      <c r="C76" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C76" s="60"/>
-      <c r="D76" s="60"/>
-      <c r="E76" s="61" t="s">
+      <c r="D76" s="74"/>
+      <c r="E76" s="75"/>
+      <c r="F76" s="75"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="75"/>
+      <c r="I76" s="76" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="55"/>
-      <c r="E77" s="54" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="55"/>
-      <c r="E78" s="54" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="55"/>
-      <c r="E79" s="54" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="55"/>
-      <c r="B80" s="56"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="57" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="55"/>
-      <c r="B81" s="60" t="s">
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="58"/>
+      <c r="B77" s="64"/>
+      <c r="H77" s="62"/>
+      <c r="I77" s="63" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="58"/>
+      <c r="B78" s="64"/>
+      <c r="H78" s="62"/>
+      <c r="I78" s="63" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="58"/>
+      <c r="B79" s="64"/>
+      <c r="H79" s="62"/>
+      <c r="I79" s="63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="58"/>
+      <c r="B80" s="65"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66"/>
+      <c r="H80" s="66"/>
+      <c r="I80" s="67" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="58"/>
+      <c r="B81" s="65"/>
+      <c r="C81" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C81" s="67" t="s">
+      <c r="D81" s="94"/>
+      <c r="E81" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="D81" s="60"/>
-      <c r="E81" s="61" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="55"/>
-      <c r="C82" s="68"/>
-      <c r="E82" s="54" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="55"/>
-      <c r="C83" s="68"/>
-      <c r="E83" s="54" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="55"/>
-      <c r="C84" s="68"/>
-      <c r="E84" s="54" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="55"/>
-      <c r="C85" s="69"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="57" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="55"/>
-      <c r="C86" s="67" t="s">
+      <c r="F81" s="74"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="75"/>
+      <c r="I81" s="76" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="58"/>
+      <c r="B82" s="64"/>
+      <c r="D82" s="62"/>
+      <c r="E82" s="58"/>
+      <c r="H82" s="62"/>
+      <c r="I82" s="63" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="58"/>
+      <c r="B83" s="64"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="58"/>
+      <c r="H83" s="62"/>
+      <c r="I83" s="63" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="58"/>
+      <c r="B84" s="64"/>
+      <c r="D84" s="62"/>
+      <c r="E84" s="58"/>
+      <c r="H84" s="62"/>
+      <c r="I84" s="63" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="58"/>
+      <c r="B85" s="64"/>
+      <c r="D85" s="62"/>
+      <c r="E85" s="96"/>
+      <c r="F85" s="66"/>
+      <c r="G85" s="66"/>
+      <c r="H85" s="66"/>
+      <c r="I85" s="67" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="58"/>
+      <c r="B86" s="64"/>
+      <c r="D86" s="60"/>
+      <c r="E86" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="D86" s="60"/>
-      <c r="E86" s="61" t="s">
+      <c r="F86" s="74"/>
+      <c r="G86" s="75"/>
+      <c r="H86" s="75"/>
+      <c r="I86" s="76" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="55"/>
-      <c r="C87" s="70"/>
-      <c r="E87" s="54" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="55"/>
-      <c r="C88" s="68"/>
-      <c r="E88" s="54" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="55"/>
-      <c r="C89" s="68"/>
-      <c r="E89" s="54" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="55"/>
-      <c r="B90" s="61" t="s">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="58"/>
+      <c r="B87" s="64"/>
+      <c r="D87" s="60"/>
+      <c r="E87" s="97"/>
+      <c r="H87" s="62"/>
+      <c r="I87" s="63" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="58"/>
+      <c r="B88" s="64"/>
+      <c r="D88" s="62"/>
+      <c r="E88" s="58"/>
+      <c r="H88" s="62"/>
+      <c r="I88" s="63" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="58"/>
+      <c r="B89" s="64"/>
+      <c r="D89" s="62"/>
+      <c r="E89" s="58"/>
+      <c r="H89" s="62"/>
+      <c r="I89" s="63" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="58"/>
+      <c r="B90" s="65"/>
+      <c r="C90" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C90" s="59" t="s">
+      <c r="D90" s="59"/>
+      <c r="E90" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="60"/>
-      <c r="E90" s="61" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="55"/>
-      <c r="B91" s="54"/>
-      <c r="E91" s="54" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="55"/>
-      <c r="B92" s="54"/>
-      <c r="E92" s="54" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="55"/>
-      <c r="B93" s="54"/>
-      <c r="E93" s="54" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="55"/>
-      <c r="B94" s="54"/>
-      <c r="E94" s="54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="55"/>
-      <c r="B95" s="54"/>
-      <c r="E95" s="54" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="55"/>
-      <c r="B96" s="54"/>
-      <c r="E96" s="54" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="55"/>
-      <c r="B97" s="54"/>
-      <c r="E97" s="54" t="s">
+      <c r="F90" s="74"/>
+      <c r="G90" s="75"/>
+      <c r="H90" s="75"/>
+      <c r="I90" s="76" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="55"/>
-      <c r="B98" s="54"/>
-      <c r="E98" s="54" t="s">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="58"/>
+      <c r="B91" s="65"/>
+      <c r="C91" s="62"/>
+      <c r="D91" s="64"/>
+      <c r="H91" s="62"/>
+      <c r="I91" s="63" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="55"/>
-      <c r="B99" s="54"/>
-      <c r="C99" s="56"/>
-      <c r="D99" s="56"/>
-      <c r="E99" s="57" t="s">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="58"/>
+      <c r="B92" s="65"/>
+      <c r="C92" s="62"/>
+      <c r="D92" s="64"/>
+      <c r="H92" s="62"/>
+      <c r="I92" s="63" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="55"/>
-      <c r="B100" s="54"/>
-      <c r="C100" s="60" t="s">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="58"/>
+      <c r="B93" s="65"/>
+      <c r="C93" s="62"/>
+      <c r="D93" s="64"/>
+      <c r="H93" s="62"/>
+      <c r="I93" s="63" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="58"/>
+      <c r="B94" s="65"/>
+      <c r="C94" s="62"/>
+      <c r="D94" s="64"/>
+      <c r="H94" s="62"/>
+      <c r="I94" s="63" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="58"/>
+      <c r="B95" s="65"/>
+      <c r="C95" s="62"/>
+      <c r="D95" s="64"/>
+      <c r="H95" s="62"/>
+      <c r="I95" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="58"/>
+      <c r="B96" s="65"/>
+      <c r="C96" s="62"/>
+      <c r="D96" s="64"/>
+      <c r="H96" s="62"/>
+      <c r="I96" s="63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="58"/>
+      <c r="B97" s="65"/>
+      <c r="C97" s="62"/>
+      <c r="D97" s="64"/>
+      <c r="H97" s="62"/>
+      <c r="I97" s="63" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="58"/>
+      <c r="B98" s="65"/>
+      <c r="C98" s="62"/>
+      <c r="D98" s="64"/>
+      <c r="H98" s="62"/>
+      <c r="I98" s="63" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="58"/>
+      <c r="B99" s="65"/>
+      <c r="C99" s="62"/>
+      <c r="D99" s="65"/>
+      <c r="E99" s="66"/>
+      <c r="F99" s="66"/>
+      <c r="G99" s="66"/>
+      <c r="H99" s="66"/>
+      <c r="I99" s="67" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="58"/>
+      <c r="B100" s="65"/>
+      <c r="C100" s="62"/>
+      <c r="D100" s="65"/>
+      <c r="E100" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="D100" s="67" t="s">
+      <c r="F100" s="74"/>
+      <c r="G100" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="E100" s="61" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="55"/>
-      <c r="B101" s="54"/>
-      <c r="D101" s="68"/>
-      <c r="E101" s="54" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="55"/>
-      <c r="B102" s="54"/>
-      <c r="D102" s="68"/>
-      <c r="E102" s="54" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="55"/>
-      <c r="B103" s="54"/>
-      <c r="D103" s="67" t="s">
+      <c r="H100" s="74"/>
+      <c r="I100" s="76" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="58"/>
+      <c r="B101" s="65"/>
+      <c r="C101" s="62"/>
+      <c r="D101" s="64"/>
+      <c r="F101" s="62"/>
+      <c r="G101" s="58"/>
+      <c r="H101" s="62"/>
+      <c r="I101" s="63" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="58"/>
+      <c r="B102" s="65"/>
+      <c r="C102" s="62"/>
+      <c r="D102" s="64"/>
+      <c r="F102" s="62"/>
+      <c r="G102" s="58"/>
+      <c r="H102" s="62"/>
+      <c r="I102" s="63" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="58"/>
+      <c r="B103" s="65"/>
+      <c r="C103" s="62"/>
+      <c r="D103" s="64"/>
+      <c r="F103" s="60"/>
+      <c r="G103" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="E103" s="61" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="55"/>
-      <c r="B104" s="54"/>
-      <c r="D104" s="68"/>
-      <c r="E104" s="54" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="55"/>
-      <c r="B105" s="54"/>
-      <c r="D105" s="68"/>
-      <c r="E105" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="55"/>
-      <c r="B106" s="54"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="57" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="55"/>
-      <c r="B107" s="54"/>
-      <c r="C107" s="61" t="s">
+      <c r="H103" s="74"/>
+      <c r="I103" s="76" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="58"/>
+      <c r="B104" s="65"/>
+      <c r="C104" s="62"/>
+      <c r="D104" s="64"/>
+      <c r="F104" s="62"/>
+      <c r="G104" s="58"/>
+      <c r="H104" s="62"/>
+      <c r="I104" s="63" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="58"/>
+      <c r="B105" s="65"/>
+      <c r="C105" s="62"/>
+      <c r="D105" s="64"/>
+      <c r="F105" s="62"/>
+      <c r="G105" s="58"/>
+      <c r="H105" s="62"/>
+      <c r="I105" s="63" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="58"/>
+      <c r="B106" s="65"/>
+      <c r="C106" s="62"/>
+      <c r="D106" s="64"/>
+      <c r="F106" s="62"/>
+      <c r="G106" s="96"/>
+      <c r="H106" s="66"/>
+      <c r="I106" s="67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="58"/>
+      <c r="B107" s="65"/>
+      <c r="C107" s="62"/>
+      <c r="D107" s="65"/>
+      <c r="E107" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="D107" s="53" t="s">
+      <c r="F107" s="74"/>
+      <c r="G107" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="E107" s="54" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="55"/>
-      <c r="B108" s="54"/>
-      <c r="C108" s="54"/>
-      <c r="E108" s="54" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="55"/>
-      <c r="B109" s="54"/>
-      <c r="C109" s="54"/>
-      <c r="E109" s="54" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="55"/>
-      <c r="B110" s="54"/>
-      <c r="C110" s="54"/>
-      <c r="D110" s="56"/>
-      <c r="E110" s="57" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="55"/>
-      <c r="B111" s="54"/>
-      <c r="C111" s="54"/>
-      <c r="D111" s="59" t="s">
+      <c r="H107" s="74"/>
+      <c r="I107" s="63" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="58"/>
+      <c r="B108" s="65"/>
+      <c r="C108" s="62"/>
+      <c r="D108" s="65"/>
+      <c r="E108" s="62"/>
+      <c r="F108" s="64"/>
+      <c r="H108" s="62"/>
+      <c r="I108" s="63" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="58"/>
+      <c r="B109" s="65"/>
+      <c r="C109" s="62"/>
+      <c r="D109" s="65"/>
+      <c r="E109" s="62"/>
+      <c r="F109" s="64"/>
+      <c r="H109" s="62"/>
+      <c r="I109" s="63" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="58"/>
+      <c r="B110" s="65"/>
+      <c r="C110" s="62"/>
+      <c r="D110" s="65"/>
+      <c r="E110" s="62"/>
+      <c r="F110" s="65"/>
+      <c r="G110" s="66"/>
+      <c r="H110" s="66"/>
+      <c r="I110" s="67" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="58"/>
+      <c r="B111" s="65"/>
+      <c r="C111" s="62"/>
+      <c r="D111" s="65"/>
+      <c r="E111" s="62"/>
+      <c r="F111" s="68"/>
+      <c r="G111" s="73" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="55"/>
-      <c r="B112" s="54"/>
-      <c r="C112" s="54"/>
-    </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="55"/>
-      <c r="B113" s="54"/>
-      <c r="C113" s="54"/>
-      <c r="E113" s="54" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="55"/>
-      <c r="B114" s="54"/>
-      <c r="C114" s="54"/>
-      <c r="E114" s="54" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="55"/>
-      <c r="B115" s="54"/>
-      <c r="C115" s="57"/>
-      <c r="D115" s="56"/>
-      <c r="E115" s="57" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="55"/>
-      <c r="B116" s="54"/>
-      <c r="C116" s="58" t="s">
+      <c r="H111" s="74"/>
+      <c r="I111" s="63" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="58"/>
+      <c r="B112" s="65"/>
+      <c r="C112" s="62"/>
+      <c r="D112" s="65"/>
+      <c r="E112" s="62"/>
+      <c r="F112" s="64"/>
+      <c r="I112" s="63" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="58"/>
+      <c r="B113" s="65"/>
+      <c r="C113" s="62"/>
+      <c r="D113" s="65"/>
+      <c r="E113" s="62"/>
+      <c r="F113" s="64"/>
+      <c r="H113" s="62"/>
+      <c r="I113" s="67" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="58"/>
+      <c r="B114" s="65"/>
+      <c r="C114" s="62"/>
+      <c r="D114" s="68"/>
+      <c r="E114" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D116" s="2"/>
-      <c r="E116" s="3" t="s">
+      <c r="F114" s="98"/>
+      <c r="G114" s="71"/>
+      <c r="H114" s="71"/>
+      <c r="I114" s="72" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="55"/>
-      <c r="B117" s="54"/>
-      <c r="C117" s="71" t="s">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="58"/>
+      <c r="B115" s="65"/>
+      <c r="C115" s="62"/>
+      <c r="D115" s="68"/>
+      <c r="E115" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="D117" s="56"/>
-      <c r="E117" s="57" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="55"/>
-      <c r="B118" s="54"/>
-      <c r="C118" s="61" t="s">
+      <c r="F115" s="98"/>
+      <c r="G115" s="66"/>
+      <c r="H115" s="66"/>
+      <c r="I115" s="67" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="58"/>
+      <c r="B116" s="65"/>
+      <c r="C116" s="62"/>
+      <c r="D116" s="65"/>
+      <c r="E116" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="D118" s="67" t="s">
+      <c r="F116" s="94"/>
+      <c r="G116" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="E118" s="61" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="55"/>
-      <c r="B119" s="54"/>
-      <c r="C119" s="54"/>
-      <c r="D119" s="72"/>
-      <c r="E119" s="57" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="55"/>
-      <c r="B120" s="54"/>
-      <c r="C120" s="54"/>
-      <c r="D120" s="73" t="s">
+      <c r="H116" s="74"/>
+      <c r="I116" s="76" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="58"/>
+      <c r="B117" s="65"/>
+      <c r="C117" s="62"/>
+      <c r="D117" s="65"/>
+      <c r="E117" s="65"/>
+      <c r="F117" s="60"/>
+      <c r="G117" s="101"/>
+      <c r="H117" s="66"/>
+      <c r="I117" s="67" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="58"/>
+      <c r="B118" s="65"/>
+      <c r="C118" s="62"/>
+      <c r="D118" s="65"/>
+      <c r="E118" s="65"/>
+      <c r="F118" s="60"/>
+      <c r="G118" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="E120" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="55"/>
-      <c r="B121" s="54"/>
-      <c r="C121" s="54"/>
-      <c r="D121" s="73" t="s">
+      <c r="H118" s="70"/>
+      <c r="I118" s="72" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="58"/>
+      <c r="B119" s="65"/>
+      <c r="C119" s="62"/>
+      <c r="D119" s="65"/>
+      <c r="E119" s="65"/>
+      <c r="F119" s="60"/>
+      <c r="G119" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="E121" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="55"/>
-      <c r="B122" s="54"/>
-      <c r="C122" s="54"/>
-      <c r="D122" s="67" t="s">
+      <c r="H119" s="70"/>
+      <c r="I119" s="72" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="58"/>
+      <c r="B120" s="65"/>
+      <c r="C120" s="62"/>
+      <c r="D120" s="65"/>
+      <c r="E120" s="65"/>
+      <c r="F120" s="60"/>
+      <c r="G120" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="E122" s="61" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="55"/>
-      <c r="B123" s="54"/>
-      <c r="C123" s="54"/>
-      <c r="D123" s="70"/>
-      <c r="E123" s="54" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="55"/>
-      <c r="B124" s="54"/>
-      <c r="C124" s="54"/>
-      <c r="D124" s="70"/>
-      <c r="E124" s="54" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="125" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="55"/>
-      <c r="B125" s="54"/>
-      <c r="C125" s="54"/>
-      <c r="D125" s="72"/>
-      <c r="E125" s="57" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="55"/>
-      <c r="B126" s="54"/>
-      <c r="C126" s="54"/>
-      <c r="D126" s="67" t="s">
+      <c r="H120" s="74"/>
+      <c r="I120" s="76" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="58"/>
+      <c r="B121" s="65"/>
+      <c r="C121" s="62"/>
+      <c r="D121" s="65"/>
+      <c r="E121" s="65"/>
+      <c r="F121" s="60"/>
+      <c r="G121" s="97"/>
+      <c r="H121" s="62"/>
+      <c r="I121" s="63" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="58"/>
+      <c r="B122" s="65"/>
+      <c r="C122" s="62"/>
+      <c r="D122" s="65"/>
+      <c r="E122" s="65"/>
+      <c r="F122" s="60"/>
+      <c r="G122" s="97"/>
+      <c r="H122" s="62"/>
+      <c r="I122" s="63" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="58"/>
+      <c r="B123" s="65"/>
+      <c r="C123" s="62"/>
+      <c r="D123" s="65"/>
+      <c r="E123" s="65"/>
+      <c r="F123" s="60"/>
+      <c r="G123" s="101"/>
+      <c r="H123" s="66"/>
+      <c r="I123" s="67" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="58"/>
+      <c r="B124" s="65"/>
+      <c r="C124" s="62"/>
+      <c r="D124" s="65"/>
+      <c r="E124" s="65"/>
+      <c r="F124" s="60"/>
+      <c r="G124" s="95" t="s">
         <v>40</v>
       </c>
-      <c r="E126" s="61" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="55"/>
-      <c r="B127" s="54"/>
-      <c r="C127" s="57"/>
-      <c r="D127" s="69"/>
-      <c r="E127" s="57" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="55"/>
-      <c r="B128" s="54"/>
-      <c r="C128" s="59" t="s">
+      <c r="H124" s="74"/>
+      <c r="I124" s="76" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="58"/>
+      <c r="B125" s="65"/>
+      <c r="C125" s="62"/>
+      <c r="D125" s="65"/>
+      <c r="E125" s="93"/>
+      <c r="F125" s="66"/>
+      <c r="G125" s="96"/>
+      <c r="H125" s="66"/>
+      <c r="I125" s="67" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="58"/>
+      <c r="B126" s="65"/>
+      <c r="C126" s="62"/>
+      <c r="D126" s="68"/>
+      <c r="E126" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="D128" s="60"/>
-      <c r="E128" s="61" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="55"/>
-      <c r="B129" s="54"/>
-      <c r="E129" s="54" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="55"/>
-      <c r="B130" s="54"/>
-      <c r="E130" s="54" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="55"/>
-      <c r="B131" s="54"/>
-      <c r="E131" s="54" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="55"/>
-      <c r="B132" s="54"/>
-      <c r="E132" s="54" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="55"/>
-      <c r="B133" s="54"/>
-      <c r="E133" s="54" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="55"/>
-      <c r="B134" s="54"/>
-      <c r="E134" s="54" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="55"/>
-      <c r="B135" s="54"/>
-      <c r="E135" s="54" t="s">
+      <c r="F126" s="74"/>
+      <c r="G126" s="75"/>
+      <c r="H126" s="75"/>
+      <c r="I126" s="76" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="55"/>
-      <c r="B136" s="54"/>
-      <c r="E136" s="54" t="s">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="58"/>
+      <c r="B127" s="65"/>
+      <c r="C127" s="62"/>
+      <c r="D127" s="64"/>
+      <c r="H127" s="62"/>
+      <c r="I127" s="63" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="55"/>
-      <c r="B137" s="54"/>
-      <c r="C137" s="59" t="s">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="58"/>
+      <c r="B128" s="65"/>
+      <c r="C128" s="62"/>
+      <c r="D128" s="64"/>
+      <c r="H128" s="62"/>
+      <c r="I128" s="63" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="58"/>
+      <c r="B129" s="65"/>
+      <c r="C129" s="62"/>
+      <c r="D129" s="64"/>
+      <c r="H129" s="62"/>
+      <c r="I129" s="63" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="58"/>
+      <c r="B130" s="65"/>
+      <c r="C130" s="62"/>
+      <c r="D130" s="64"/>
+      <c r="H130" s="62"/>
+      <c r="I130" s="63" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="58"/>
+      <c r="B131" s="65"/>
+      <c r="C131" s="62"/>
+      <c r="D131" s="64"/>
+      <c r="H131" s="62"/>
+      <c r="I131" s="63" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="58"/>
+      <c r="B132" s="65"/>
+      <c r="C132" s="62"/>
+      <c r="D132" s="64"/>
+      <c r="H132" s="62"/>
+      <c r="I132" s="63" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="58"/>
+      <c r="B133" s="65"/>
+      <c r="C133" s="62"/>
+      <c r="D133" s="64"/>
+      <c r="H133" s="62"/>
+      <c r="I133" s="63" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="58"/>
+      <c r="B134" s="65"/>
+      <c r="C134" s="62"/>
+      <c r="D134" s="64"/>
+      <c r="H134" s="62"/>
+      <c r="I134" s="63" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="58"/>
+      <c r="B135" s="65"/>
+      <c r="C135" s="62"/>
+      <c r="D135" s="68"/>
+      <c r="E135" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="D137" s="60"/>
-      <c r="E137" s="61" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="55"/>
-      <c r="B138" s="54"/>
-      <c r="E138" s="54" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="55"/>
-      <c r="B139" s="54"/>
-      <c r="E139" s="54" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="55"/>
-      <c r="B140" s="54"/>
-      <c r="C140" s="56"/>
-      <c r="D140" s="56"/>
-      <c r="E140" s="57" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="55"/>
-      <c r="B141" s="54"/>
-      <c r="C141" s="53" t="s">
+      <c r="F135" s="74"/>
+      <c r="G135" s="75"/>
+      <c r="H135" s="75"/>
+      <c r="I135" s="76" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="58"/>
+      <c r="B136" s="65"/>
+      <c r="C136" s="62"/>
+      <c r="D136" s="64"/>
+      <c r="H136" s="62"/>
+      <c r="I136" s="63" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="58"/>
+      <c r="B137" s="65"/>
+      <c r="C137" s="62"/>
+      <c r="D137" s="64"/>
+      <c r="H137" s="62"/>
+      <c r="I137" s="63" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="58"/>
+      <c r="B138" s="65"/>
+      <c r="C138" s="62"/>
+      <c r="D138" s="65"/>
+      <c r="E138" s="66"/>
+      <c r="F138" s="66"/>
+      <c r="G138" s="66"/>
+      <c r="H138" s="66"/>
+      <c r="I138" s="67" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="58"/>
+      <c r="B139" s="65"/>
+      <c r="C139" s="62"/>
+      <c r="D139" s="68"/>
+      <c r="E139" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="E141" s="54" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="55"/>
-      <c r="B142" s="57"/>
-      <c r="E142" s="54" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="55"/>
-      <c r="B143" s="0" t="s">
+      <c r="F139" s="61"/>
+      <c r="H139" s="62"/>
+      <c r="I139" s="63" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="58"/>
+      <c r="B140" s="65"/>
+      <c r="C140" s="66"/>
+      <c r="D140" s="103"/>
+      <c r="H140" s="62"/>
+      <c r="I140" s="63" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="58"/>
+      <c r="B141" s="64"/>
+      <c r="C141" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C143" s="67" t="s">
+      <c r="D141" s="104"/>
+      <c r="E141" s="95" t="s">
         <v>45</v>
       </c>
+      <c r="F141" s="74"/>
+      <c r="G141" s="75"/>
+      <c r="H141" s="75"/>
+      <c r="I141" s="76" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="58"/>
+      <c r="B142" s="64"/>
+      <c r="D142" s="60"/>
+      <c r="E142" s="97"/>
+      <c r="H142" s="62"/>
+      <c r="I142" s="63" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="58"/>
+      <c r="B143" s="64"/>
       <c r="D143" s="60"/>
-      <c r="E143" s="61" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="55"/>
-      <c r="C144" s="70"/>
-      <c r="E144" s="54" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="55"/>
-      <c r="C145" s="72"/>
-      <c r="D145" s="56"/>
-      <c r="E145" s="57" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="55"/>
-      <c r="C146" s="67" t="s">
+      <c r="E143" s="101"/>
+      <c r="F143" s="66"/>
+      <c r="G143" s="66"/>
+      <c r="H143" s="66"/>
+      <c r="I143" s="67" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="58"/>
+      <c r="B144" s="64"/>
+      <c r="D144" s="60"/>
+      <c r="E144" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="D146" s="60"/>
-      <c r="E146" s="61" t="s">
+      <c r="F144" s="74"/>
+      <c r="G144" s="75"/>
+      <c r="H144" s="75"/>
+      <c r="I144" s="76" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="55"/>
-      <c r="B147" s="56"/>
-      <c r="C147" s="69"/>
-      <c r="D147" s="71"/>
-      <c r="E147" s="57" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="55"/>
-      <c r="B148" s="59" t="s">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="58"/>
+      <c r="B145" s="65"/>
+      <c r="C145" s="66"/>
+      <c r="D145" s="66"/>
+      <c r="E145" s="96"/>
+      <c r="F145" s="99"/>
+      <c r="G145" s="99"/>
+      <c r="H145" s="66"/>
+      <c r="I145" s="67" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="58"/>
+      <c r="B146" s="68"/>
+      <c r="C146" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="C148" s="60"/>
-      <c r="D148" s="59"/>
-      <c r="E148" s="61" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="55"/>
-      <c r="E149" s="54" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="55"/>
-      <c r="E150" s="54" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="55"/>
-      <c r="E151" s="54" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="55"/>
-      <c r="E152" s="54" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="55"/>
-      <c r="E153" s="54" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="55"/>
-      <c r="E154" s="54" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="55"/>
-      <c r="E155" s="54" t="s">
+      <c r="D146" s="74"/>
+      <c r="E146" s="75"/>
+      <c r="F146" s="73"/>
+      <c r="G146" s="73"/>
+      <c r="H146" s="75"/>
+      <c r="I146" s="76" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="55"/>
-      <c r="E156" s="54" t="s">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="58"/>
+      <c r="B147" s="64"/>
+      <c r="H147" s="62"/>
+      <c r="I147" s="63" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="55"/>
-      <c r="D157" s="53"/>
-      <c r="E157" s="54" t="s">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="58"/>
+      <c r="B148" s="64"/>
+      <c r="H148" s="62"/>
+      <c r="I148" s="63" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="55"/>
-      <c r="E158" s="54" t="s">
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="58"/>
+      <c r="B149" s="64"/>
+      <c r="H149" s="62"/>
+      <c r="I149" s="63" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="55"/>
-      <c r="D159" s="53"/>
-      <c r="E159" s="54" t="s">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="58"/>
+      <c r="B150" s="64"/>
+      <c r="H150" s="62"/>
+      <c r="I150" s="63" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="55"/>
-      <c r="E160" s="54" t="s">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="58"/>
+      <c r="B151" s="64"/>
+      <c r="H151" s="62"/>
+      <c r="I151" s="63" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="55"/>
-      <c r="D161" s="53"/>
-      <c r="E161" s="54" t="s">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="58"/>
+      <c r="B152" s="64"/>
+      <c r="H152" s="62"/>
+      <c r="I152" s="63" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="55"/>
-      <c r="E162" s="74" t="s">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="58"/>
+      <c r="B153" s="64"/>
+      <c r="H153" s="62"/>
+      <c r="I153" s="63" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="55"/>
-      <c r="E163" s="74" t="s">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="58"/>
+      <c r="B154" s="64"/>
+      <c r="H154" s="62"/>
+      <c r="I154" s="63" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="55"/>
-      <c r="E164" s="74" t="s">
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="58"/>
+      <c r="B155" s="64"/>
+      <c r="F155" s="60"/>
+      <c r="G155" s="60"/>
+      <c r="H155" s="62"/>
+      <c r="I155" s="63" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="55"/>
-      <c r="E165" s="74" t="s">
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="58"/>
+      <c r="B156" s="64"/>
+      <c r="H156" s="62"/>
+      <c r="I156" s="63" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="55"/>
-      <c r="E166" s="54" t="s">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="58"/>
+      <c r="B157" s="64"/>
+      <c r="F157" s="60"/>
+      <c r="G157" s="60"/>
+      <c r="H157" s="62"/>
+      <c r="I157" s="63" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="55"/>
-      <c r="E167" s="54" t="s">
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="58"/>
+      <c r="B158" s="64"/>
+      <c r="H158" s="62"/>
+      <c r="I158" s="63" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="55"/>
-      <c r="E168" s="54" t="s">
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="58"/>
+      <c r="B159" s="64"/>
+      <c r="F159" s="60"/>
+      <c r="G159" s="60"/>
+      <c r="H159" s="62"/>
+      <c r="I159" s="63" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="55"/>
-      <c r="E169" s="54" t="s">
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="58"/>
+      <c r="B160" s="64"/>
+      <c r="H160" s="105"/>
+      <c r="I160" s="106" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="55"/>
-      <c r="E170" s="54" t="s">
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="58"/>
+      <c r="B161" s="64"/>
+      <c r="H161" s="105"/>
+      <c r="I161" s="106" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="55"/>
-      <c r="E171" s="54" t="s">
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="58"/>
+      <c r="B162" s="64"/>
+      <c r="H162" s="105"/>
+      <c r="I162" s="106" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="55"/>
-      <c r="E172" s="54" t="s">
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="58"/>
+      <c r="B163" s="64"/>
+      <c r="H163" s="105"/>
+      <c r="I163" s="106" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="55"/>
-      <c r="E173" s="54" t="s">
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="58"/>
+      <c r="B164" s="64"/>
+      <c r="H164" s="62"/>
+      <c r="I164" s="63" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="55"/>
-      <c r="E174" s="54" t="s">
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="58"/>
+      <c r="B165" s="64"/>
+      <c r="H165" s="62"/>
+      <c r="I165" s="63" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="55"/>
-      <c r="E175" s="54" t="s">
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="58"/>
+      <c r="B166" s="64"/>
+      <c r="H166" s="62"/>
+      <c r="I166" s="63" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="55"/>
-      <c r="E176" s="54" t="s">
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="58"/>
+      <c r="B167" s="64"/>
+      <c r="H167" s="62"/>
+      <c r="I167" s="63" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="55"/>
-      <c r="E177" s="54" t="s">
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="58"/>
+      <c r="B168" s="64"/>
+      <c r="H168" s="62"/>
+      <c r="I168" s="63" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="55"/>
-      <c r="E178" s="54" t="s">
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="58"/>
+      <c r="B169" s="64"/>
+      <c r="H169" s="62"/>
+      <c r="I169" s="63" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="55"/>
-      <c r="E179" s="54" t="s">
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="58"/>
+      <c r="B170" s="64"/>
+      <c r="H170" s="62"/>
+      <c r="I170" s="63" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="55"/>
-      <c r="B180" s="59" t="s">
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="58"/>
+      <c r="B171" s="64"/>
+      <c r="H171" s="62"/>
+      <c r="I171" s="63" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="58"/>
+      <c r="B172" s="64"/>
+      <c r="H172" s="62"/>
+      <c r="I172" s="63" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="58"/>
+      <c r="B173" s="64"/>
+      <c r="H173" s="62"/>
+      <c r="I173" s="63" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="58"/>
+      <c r="B174" s="64"/>
+      <c r="H174" s="62"/>
+      <c r="I174" s="63" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="58"/>
+      <c r="B175" s="64"/>
+      <c r="H175" s="62"/>
+      <c r="I175" s="63" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="58"/>
+      <c r="B176" s="64"/>
+      <c r="H176" s="62"/>
+      <c r="I176" s="63" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="58"/>
+      <c r="B177" s="64"/>
+      <c r="H177" s="62"/>
+      <c r="I177" s="63" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="58"/>
+      <c r="B178" s="68"/>
+      <c r="C178" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="C180" s="60"/>
-      <c r="D180" s="60"/>
-      <c r="E180" s="61" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="55"/>
-      <c r="E181" s="54" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="55"/>
-      <c r="E182" s="54" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="55"/>
-      <c r="E183" s="54" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="55"/>
-      <c r="E184" s="54" t="s">
-        <v>337</v>
+      <c r="D178" s="74"/>
+      <c r="E178" s="75"/>
+      <c r="F178" s="75"/>
+      <c r="G178" s="75"/>
+      <c r="H178" s="75"/>
+      <c r="I178" s="76" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="58"/>
+      <c r="B179" s="64"/>
+      <c r="H179" s="62"/>
+      <c r="I179" s="63" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="58"/>
+      <c r="B180" s="64"/>
+      <c r="H180" s="62"/>
+      <c r="I180" s="63" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="58"/>
+      <c r="B181" s="64"/>
+      <c r="H181" s="62"/>
+      <c r="I181" s="63" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="58"/>
+      <c r="B182" s="64"/>
+      <c r="H182" s="62"/>
+      <c r="I182" s="63" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="58"/>
+      <c r="B183" s="64"/>
+      <c r="H183" s="62"/>
+      <c r="I183" s="63" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="96"/>
+      <c r="B184" s="93"/>
+      <c r="C184" s="66"/>
+      <c r="D184" s="66"/>
+      <c r="E184" s="66"/>
+      <c r="F184" s="66"/>
+      <c r="G184" s="66"/>
+      <c r="H184" s="66"/>
+      <c r="I184" s="67" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="55"/>
-      <c r="E185" s="54" t="s">
-        <v>338</v>
+      <c r="A185" s="107"/>
+      <c r="E185" s="108" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="75"/>
-      <c r="B186" s="56"/>
-      <c r="C186" s="56"/>
-      <c r="D186" s="56"/>
-      <c r="E186" s="57" t="s">
-        <v>339</v>
+      <c r="A186" s="109"/>
+      <c r="B186" s="110"/>
+      <c r="C186" s="110"/>
+      <c r="D186" s="110"/>
+      <c r="E186" s="111" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>